<commit_message>
view and delete HR
</commit_message>
<xml_diff>
--- a/src/main/webapp/Data_Dictionary/Data_Dictionary.xlsx
+++ b/src/main/webapp/Data_Dictionary/Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansi\eclipse-workspace\Resource_Management\src\main\webapp\Data_Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F957596-983B-4D32-8E9A-92AD610D57D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBEB486-C460-439C-A0EE-FBE89E874477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FDE8AA0-6948-4BD0-9A13-29F2E8387166}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
   <si>
     <t>Field</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>hrJoinDate</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
 </sst>
 </file>
@@ -602,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E416F30-E458-4801-BA31-F0A7A0063210}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="109" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +615,7 @@
     <col min="10" max="10" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>51</v>
       </c>
@@ -629,19 +626,19 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="4" t="s">
         <v>52</v>
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
     </row>
-    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -655,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -666,8 +663,12 @@
         <v>7</v>
       </c>
       <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -678,8 +679,20 @@
         <v>8</v>
       </c>
       <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -690,8 +703,17 @@
         <v>8</v>
       </c>
       <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -702,120 +724,89 @@
         <v>8</v>
       </c>
       <c r="D10" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
+      <c r="H10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
+      <c r="H12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
+      <c r="H13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+      <c r="I14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="1" t="s">
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G16" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+      <c r="H16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -829,7 +820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -841,7 +832,7 @@
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -853,7 +844,7 @@
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -865,7 +856,7 @@
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -877,7 +868,7 @@
       </c>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -889,7 +880,7 @@
       </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>24</v>
       </c>
@@ -903,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
@@ -917,7 +908,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1219,7 +1210,7 @@
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="G7:H7"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="G39:H39"/>

</xml_diff>

<commit_message>
Add and show Resource
</commit_message>
<xml_diff>
--- a/src/main/webapp/Data_Dictionary/Data_Dictionary.xlsx
+++ b/src/main/webapp/Data_Dictionary/Data_Dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mansi\eclipse-workspace\Resource_Management\src\main\webapp\Data_Dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBEB486-C460-439C-A0EE-FBE89E874477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E379F9D4-BBF3-4E43-9DEA-45051CA0F8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3FDE8AA0-6948-4BD0-9A13-29F2E8387166}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="59">
   <si>
     <t>Field</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Technologies name</t>
   </si>
   <si>
-    <t>Table: Database</t>
-  </si>
-  <si>
     <t>dbId</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>Table: Hr</t>
   </si>
   <si>
-    <t>Table: User</t>
-  </si>
-  <si>
     <t>Table: User_Language</t>
   </si>
   <si>
@@ -208,6 +202,15 @@
   </si>
   <si>
     <t>hrJoinDate</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Table: Databases</t>
+  </si>
+  <si>
+    <t>Table: Resource</t>
   </si>
 </sst>
 </file>
@@ -599,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E416F30-E458-4801-BA31-F0A7A0063210}">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="109" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="109" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,7 +620,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -628,7 +631,7 @@
     </row>
     <row r="2" spans="1:10" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -664,7 +667,7 @@
       </c>
       <c r="D7" s="1"/>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7" s="3"/>
     </row>
@@ -725,7 +728,7 @@
       </c>
       <c r="D10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>6</v>
@@ -736,7 +739,7 @@
     </row>
     <row r="11" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G11" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>6</v>
@@ -769,10 +772,10 @@
     </row>
     <row r="14" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>8</v>
@@ -791,7 +794,7 @@
     </row>
     <row r="16" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>6</v>
@@ -800,13 +803,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>0</v>
       </c>
@@ -819,8 +822,12 @@
       <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
@@ -831,8 +838,12 @@
         <v>7</v>
       </c>
       <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -843,8 +854,12 @@
         <v>8</v>
       </c>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>12</v>
       </c>
@@ -855,8 +870,12 @@
         <v>8</v>
       </c>
       <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -867,8 +886,12 @@
         <v>8</v>
       </c>
       <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -879,46 +902,69 @@
         <v>8</v>
       </c>
       <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -928,7 +974,7 @@
       </c>
       <c r="B33" s="3"/>
       <c r="G33" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H33" s="3"/>
     </row>
@@ -970,7 +1016,7 @@
       </c>
       <c r="D35" s="1"/>
       <c r="G35" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>5</v>
@@ -1000,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J36" s="1"/>
     </row>
@@ -1012,7 +1058,7 @@
         <v>5</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J37" s="1"/>
     </row>
@@ -1022,7 +1068,7 @@
       </c>
       <c r="B39" s="3"/>
       <c r="G39" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H39" s="3"/>
     </row>
@@ -1064,7 +1110,7 @@
       </c>
       <c r="D41" s="1"/>
       <c r="G41" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>5</v>
@@ -1094,7 +1140,7 @@
         <v>5</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J42" s="1"/>
     </row>
@@ -1106,17 +1152,17 @@
         <v>5</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J43" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B45" s="3"/>
       <c r="G45" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H45" s="3"/>
     </row>
@@ -1148,7 +1194,7 @@
     </row>
     <row r="47" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>5</v>
@@ -1158,7 +1204,7 @@
       </c>
       <c r="D47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>5</v>
@@ -1170,7 +1216,7 @@
     </row>
     <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>6</v>
@@ -1179,7 +1225,7 @@
         <v>8</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>20</v>
@@ -1188,19 +1234,19 @@
         <v>5</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="7:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="G49" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J49" s="1"/>
     </row>

</xml_diff>